<commit_message>
fixed XML serializer that sometimes corrupts data.
</commit_message>
<xml_diff>
--- a/Database Examples/ni_test_1.xlsx
+++ b/Database Examples/ni_test_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\GIT\Ballard-Arinc-429-XML-Generator\Database Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D9B8C6C-5A54-44A5-9E2E-7CC9ECFB1080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FADFEBF-6A1B-4128-8243-6C06A46AFE1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1935" yWindow="2745" windowWidth="21600" windowHeight="12735" xr2:uid="{C4FFA9CA-FD51-49DE-890F-D5CB7111E100}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{C4FFA9CA-FD51-49DE-890F-D5CB7111E100}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1024,7 +1024,7 @@
   <dimension ref="A1:Y5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="T4" sqref="T4:T5"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>